<commit_message>
interface modification due to specification of gene mutations
</commit_message>
<xml_diff>
--- a/TWT_specification.xlsx
+++ b/TWT_specification.xlsx
@@ -494,10 +494,10 @@
     <t xml:space="preserve">Q61R </t>
   </si>
   <si>
-    <t xml:space="preserve">T50I  T50I 3UTR </t>
-  </si>
-  <si>
-    <t>Q61R Q61R   Missense_Mutation</t>
+    <t xml:space="preserve">  T50I 3UTR </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Q61R   Missense_Mutation</t>
   </si>
   <si>
     <t xml:space="preserve">Q61K </t>

</xml_diff>